<commit_message>
GH-1116: Update parse user subjects, specify phoneNo format in attachments
</commit_message>
<xml_diff>
--- a/server/assets/attachments/batch_user_data_query.xlsx
+++ b/server/assets/attachments/batch_user_data_query.xlsx
@@ -23,7 +23,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Phone #</t>
+    <t>Phone # (e.g. 12345678)</t>
   </si>
   <si>
     <t>Email</t>
@@ -102,10 +102,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -343,23 +343,23 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" ht="15.75" customHeight="1"/>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -5024,8 +5024,8 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">

</xml_diff>